<commit_message>
Tested out formulas and updated spreadsheet with variables.
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Formulas/test.xlsx
+++ b/Assets/Scripts/Formulas/test.xlsx
@@ -14,7 +14,11 @@
   <sheets>
     <sheet name="TestSheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="DEX">TestSheet!$C$2</definedName>
+    <definedName name="STR">TestSheet!$B$2</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -24,10 +28,10 @@
     <t>Wee</t>
   </si>
   <si>
-    <t>Hello</t>
+    <t>STR</t>
   </si>
   <si>
-    <t>World</t>
+    <t>DEX</t>
   </si>
 </sst>
 </file>
@@ -348,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -359,33 +363,43 @@
     <col min="1" max="26" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <f>SUM(STR, DEX)</f>
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>